<commit_message>
Probando el codigo (Version 1)
</commit_message>
<xml_diff>
--- a/storage/archivos/Preguntas.xlsx
+++ b/storage/archivos/Preguntas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Nubes\Dropbox\LOS_ETERNOS\GG\COMPDES\Archivos de Carga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter\Dropbox\DSI-215\GG\COMPDES\Archivos de Carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>PREGUNTA</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>TODAS</t>
+  </si>
+  <si>
+    <t>NINGUNA</t>
+  </si>
+  <si>
+    <t>¿Sere capaz de usar un recycler view adecuadmente?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI </t>
+  </si>
+  <si>
+    <t>NO SE</t>
+  </si>
+  <si>
+    <t>MAS O MENOS</t>
   </si>
 </sst>
 </file>
@@ -417,16 +435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,6 +508,29 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>